<commit_message>
html to pdf updated
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\analyzed-exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padidar\analyzed-exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CE66FB-EA34-444F-A617-638AA66265A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF14CD8B-9856-4ED0-B57E-50AB343C7719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1859" yWindow="1859" windowWidth="18851" windowHeight="9766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="داده ها" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">نتایج!$G$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1880,7 +1890,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -1948,7 +1958,7 @@
     <col min="217" max="238" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>177</v>
       </c>
@@ -2664,7 +2674,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29">
         <v>2</v>
       </c>
@@ -2934,7 +2944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -3648,7 +3658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>2</v>
       </c>
@@ -4366,7 +4376,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -5078,7 +5088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>2</v>
       </c>
@@ -5792,7 +5802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>2</v>
       </c>
@@ -6510,7 +6520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>2</v>
       </c>
@@ -7226,7 +7236,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -7941,7 +7951,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -8657,7 +8667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>1</v>
       </c>
@@ -9371,7 +9381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>1</v>
       </c>
@@ -10087,7 +10097,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>1</v>
       </c>
@@ -10349,7 +10359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>1</v>
       </c>
@@ -11061,7 +11071,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>2</v>
       </c>
@@ -11988,7 +11998,7 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>1</v>
       </c>
@@ -12908,7 +12918,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="17" spans="2:238" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>400</v>
       </c>
@@ -13833,11 +13843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52976ED-B169-416D-B622-CE38445F1289}">
   <dimension ref="A1:FR17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.21875" customWidth="1"/>
@@ -21181,7 +21191,7 @@
     </row>
     <row r="15" spans="1:174" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>451</v>
       </c>
       <c r="B15" t="s">
         <v>398</v>
@@ -21684,7 +21694,7 @@
     </row>
     <row r="16" spans="1:174" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>451</v>
       </c>
       <c r="B16" t="s">
         <v>399</v>
@@ -22187,7 +22197,7 @@
     </row>
     <row r="17" spans="1:174" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>175</v>
+        <v>451</v>
       </c>
       <c r="B17" t="s">
         <v>400</v>
@@ -22705,7 +22715,7 @@
       <selection pane="bottomLeft" activeCell="D14" sqref="A1:FR17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" style="24" bestFit="1" customWidth="1"/>
@@ -22774,7 +22784,7 @@
     <col min="173" max="174" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>166</v>
       </c>
@@ -23462,7 +23472,7 @@
         <v>عملکرد شغلی میانگین</v>
       </c>
     </row>
-    <row r="2" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="str">
         <f>'اطلاعات شخصی'!B2</f>
         <v>جناب آقای</v>
@@ -24160,7 +24170,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="3" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="str">
         <f>'اطلاعات شخصی'!B3</f>
         <v>جناب آقای</v>
@@ -24858,7 +24868,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="4" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="str">
         <f>'اطلاعات شخصی'!B4</f>
         <v>جناب آقای</v>
@@ -25556,7 +25566,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="5" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="str">
         <f>'اطلاعات شخصی'!B5</f>
         <v>جناب آقای</v>
@@ -26254,7 +26264,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="6" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="str">
         <f>'اطلاعات شخصی'!B6</f>
         <v>جناب آقای</v>
@@ -26952,7 +26962,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="7" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="str">
         <f>'اطلاعات شخصی'!B7</f>
         <v>جناب آقای</v>
@@ -27650,7 +27660,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="8" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="str">
         <f>'اطلاعات شخصی'!B8</f>
         <v>جناب آقای</v>
@@ -28348,7 +28358,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="9" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="str">
         <f>'اطلاعات شخصی'!B9</f>
         <v>سرکار خانم</v>
@@ -29046,7 +29056,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="10" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="str">
         <f>'اطلاعات شخصی'!B10</f>
         <v>سرکار خانم</v>
@@ -29744,7 +29754,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="11" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="str">
         <f>'اطلاعات شخصی'!B11</f>
         <v>سرکار خانم</v>
@@ -30442,7 +30452,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="12" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="str">
         <f>'اطلاعات شخصی'!B12</f>
         <v>سرکار خانم</v>
@@ -31140,7 +31150,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="13" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="str">
         <f>'اطلاعات شخصی'!B13</f>
         <v>سرکار خانم</v>
@@ -31838,7 +31848,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="14" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="str">
         <f>'اطلاعات شخصی'!B14</f>
         <v>سرکار خانم</v>
@@ -32536,7 +32546,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="15" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>175</v>
       </c>
@@ -33211,7 +33221,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="16" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>175</v>
       </c>
@@ -33886,7 +33896,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="17" spans="1:174" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>175</v>
       </c>
@@ -34575,7 +34585,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -34597,7 +34607,7 @@
     <col min="21" max="21" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -34678,7 +34688,7 @@
         <v>سن</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -34764,7 +34774,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -34850,7 +34860,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -34936,7 +34946,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -35022,7 +35032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -35108,7 +35118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -35194,7 +35204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -35280,7 +35290,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -35366,7 +35376,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -35452,7 +35462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -35538,7 +35548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -35624,7 +35634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -35710,7 +35720,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -35796,7 +35806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -35838,7 +35848,7 @@
         <v>32.571428571428569</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -35880,7 +35890,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -35939,7 +35949,7 @@
       <selection pane="bottomLeft" activeCell="O2" sqref="O2:O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -35959,7 +35969,7 @@
     <col min="31" max="52" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -36131,7 +36141,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -36339,7 +36349,7 @@
         <v>1.5144298184855884</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -36547,7 +36557,7 @@
         <v>-0.90364087837562579</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -36755,7 +36765,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -36963,7 +36973,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -37171,7 +37181,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -37379,7 +37389,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -37587,7 +37597,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -37795,7 +37805,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -38003,7 +38013,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -38211,7 +38221,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -38419,7 +38429,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -38627,7 +38637,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -38835,7 +38845,7 @@
         <v>0.28113534146345742</v>
       </c>
     </row>
-    <row r="15" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -39043,7 +39053,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -39251,7 +39261,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="17" spans="1:52" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -39476,7 +39486,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -39490,7 +39500,7 @@
     <col min="15" max="34" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -39603,7 +39613,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -39741,7 +39751,7 @@
         <v>6.5392404513888902</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -39879,7 +39889,7 @@
         <v>8.603401562500002</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -40017,7 +40027,7 @@
         <v>7.2390820312500006</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -40155,7 +40165,7 @@
         <v>9.6439869791666659</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -40293,7 +40303,7 @@
         <v>7.2198833333333345</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -40431,7 +40441,7 @@
         <v>7.0661059027777791</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -40569,7 +40579,7 @@
         <v>8.0694848958333338</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -40707,7 +40717,7 @@
         <v>7.0389062847222226</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -40845,7 +40855,7 @@
         <v>6.4232503472222238</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -40983,7 +40993,7 @@
         <v>5.8348708333333326</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -41121,7 +41131,7 @@
         <v>5.5336291666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -41259,7 +41269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -41397,7 +41407,7 @@
         <v>7.4666782986111109</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -41534,7 +41544,7 @@
         <v>9.1310507688492102</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -41671,7 +41681,7 @@
         <v>6.5945622251157419</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -41825,7 +41835,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -41844,7 +41854,7 @@
     <col min="44" max="55" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'اطلاعات شخصی'!B1</f>
         <v>جنسیت</v>
@@ -42040,7 +42050,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>'اطلاعات شخصی'!B2</f>
         <v>جناب آقای</v>
@@ -42262,7 +42272,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>'اطلاعات شخصی'!B3</f>
         <v>جناب آقای</v>
@@ -42484,7 +42494,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f>'اطلاعات شخصی'!B4</f>
         <v>جناب آقای</v>
@@ -42706,7 +42716,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f>'اطلاعات شخصی'!B5</f>
         <v>جناب آقای</v>
@@ -42928,7 +42938,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f>'اطلاعات شخصی'!B6</f>
         <v>جناب آقای</v>
@@ -43150,7 +43160,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f>'اطلاعات شخصی'!B7</f>
         <v>جناب آقای</v>
@@ -43372,7 +43382,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="8" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f>'اطلاعات شخصی'!B8</f>
         <v>جناب آقای</v>
@@ -43594,7 +43604,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="9" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f>'اطلاعات شخصی'!B9</f>
         <v>سرکار خانم</v>
@@ -43816,7 +43826,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="10" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f>'اطلاعات شخصی'!B10</f>
         <v>سرکار خانم</v>
@@ -44038,7 +44048,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="11" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f>'اطلاعات شخصی'!B11</f>
         <v>سرکار خانم</v>
@@ -44260,7 +44270,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="12" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f>'اطلاعات شخصی'!B12</f>
         <v>سرکار خانم</v>
@@ -44482,7 +44492,7 @@
         <v>شدید</v>
       </c>
     </row>
-    <row r="13" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f>'اطلاعات شخصی'!B13</f>
         <v>سرکار خانم</v>
@@ -44704,7 +44714,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="14" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f>'اطلاعات شخصی'!B14</f>
         <v>سرکار خانم</v>
@@ -44926,7 +44936,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="15" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'اطلاعات شخصی'!B15</f>
         <v>7</v>
@@ -45148,7 +45158,7 @@
         <v>14.285714285714285</v>
       </c>
     </row>
-    <row r="16" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'اطلاعات شخصی'!B16</f>
         <v>6</v>
@@ -45370,7 +45380,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="17" spans="1:55" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'اطلاعات شخصی'!B17</f>
         <v>13</v>
@@ -45606,7 +45616,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -45641,7 +45651,7 @@
     <col min="83" max="88" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -45953,7 +45963,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -46307,7 +46317,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="3" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -46661,7 +46671,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="4" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -47015,7 +47025,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="5" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -47369,7 +47379,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="6" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -47723,7 +47733,7 @@
         <v>شدید</v>
       </c>
     </row>
-    <row r="7" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -48077,7 +48087,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="8" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -48431,7 +48441,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="9" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -48785,7 +48795,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="10" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -49139,7 +49149,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="11" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -49493,7 +49503,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="12" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -49847,7 +49857,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="13" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -50201,7 +50211,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="14" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -50555,7 +50565,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="15" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -50909,7 +50919,7 @@
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="16" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -51263,7 +51273,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:88" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -51634,7 +51644,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -51665,7 +51675,7 @@
     <col min="179" max="180" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="str">
         <f>'داده ها'!CO1</f>
         <v>A1</v>
@@ -52344,7 +52354,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5">
         <f>'داده ها'!CO2</f>
         <v>0</v>
@@ -53054,7 +53064,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="3" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="5">
         <f>'داده ها'!CO3</f>
         <v>0</v>
@@ -53764,7 +53774,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="4" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="5">
         <f>'داده ها'!CO4</f>
         <v>0</v>
@@ -54474,7 +54484,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="5" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D5" s="5">
         <f>'داده ها'!CO5</f>
         <v>0</v>
@@ -55184,7 +55194,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="6" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="5">
         <f>'داده ها'!CO6</f>
         <v>0</v>
@@ -55894,7 +55904,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="7" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="5">
         <f>'داده ها'!CO7</f>
         <v>0</v>
@@ -56604,7 +56614,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="8" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="5">
         <f>'داده ها'!CO8</f>
         <v>0</v>
@@ -57314,7 +57324,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="9" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="5">
         <f>'داده ها'!CO9</f>
         <v>0</v>
@@ -58024,7 +58034,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="10" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="5">
         <f>'داده ها'!CO10</f>
         <v>0</v>
@@ -58734,7 +58744,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="11" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="5">
         <f>'داده ها'!CO11</f>
         <v>0</v>
@@ -59444,7 +59454,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="12" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="5">
         <f>'داده ها'!CO12</f>
         <v>0</v>
@@ -60154,7 +60164,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="13" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5">
         <f>'داده ها'!CO13</f>
         <v>0</v>
@@ -60864,7 +60874,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="14" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5">
         <f>'داده ها'!CO14</f>
         <v>0</v>
@@ -61574,7 +61584,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="15" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="5">
         <f t="shared" ref="D15:K15" si="31">AVERAGE(D2:D8)</f>
         <v>0</v>
@@ -62284,7 +62294,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="16" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="5">
         <f t="shared" ref="D16:K16" si="38">AVERAGE(D9:D14)</f>
         <v>0</v>
@@ -62994,7 +63004,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="17" spans="4:180" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="5">
         <f t="shared" ref="D17:K17" si="45">AVERAGE(D2:D14)</f>
         <v>0</v>

</xml_diff>

<commit_message>
Changes Aded to file1.html
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Padidar\analyzed-exercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\analyzed-exercise\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF14CD8B-9856-4ED0-B57E-50AB343C7719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDB70B1-F6F8-4E6B-8989-326588A68DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1859" yWindow="1859" windowWidth="18851" windowHeight="9766" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="داده ها" sheetId="1" r:id="rId1"/>
@@ -27,21 +27,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">نتایج!$G$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2002" uniqueCount="455">
   <si>
     <t>مجموع</t>
   </si>
@@ -1398,6 +1388,15 @@
   <si>
     <t>میانگین</t>
   </si>
+  <si>
+    <t>کارکنان آقای</t>
+  </si>
+  <si>
+    <t>کارکنان خانم</t>
+  </si>
+  <si>
+    <t>کل کارکنان</t>
+  </si>
 </sst>
 </file>
 
@@ -1890,7 +1889,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -1958,7 +1957,7 @@
     <col min="217" max="238" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="27" t="s">
         <v>177</v>
       </c>
@@ -2674,7 +2673,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29">
         <v>2</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="29">
         <v>2</v>
       </c>
@@ -3658,7 +3657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="29">
         <v>2</v>
       </c>
@@ -4376,7 +4375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -5088,7 +5087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29">
         <v>2</v>
       </c>
@@ -5802,7 +5801,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29">
         <v>2</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29">
         <v>2</v>
       </c>
@@ -7236,7 +7235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29">
         <v>1</v>
       </c>
@@ -7951,7 +7950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29">
         <v>1</v>
       </c>
@@ -8667,7 +8666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>1</v>
       </c>
@@ -9381,7 +9380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29">
         <v>1</v>
       </c>
@@ -10097,7 +10096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29">
         <v>1</v>
       </c>
@@ -10359,7 +10358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29">
         <v>1</v>
       </c>
@@ -11071,7 +11070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29">
         <v>2</v>
       </c>
@@ -11998,7 +11997,7 @@
         <v>2.8333333333333335</v>
       </c>
     </row>
-    <row r="16" spans="1:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29">
         <v>1</v>
       </c>
@@ -12918,7 +12917,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="17" spans="2:238" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:238" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>400</v>
       </c>
@@ -13844,11 +13843,13 @@
   <dimension ref="A1:FR17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.21875" customWidth="1"/>
   </cols>
@@ -21194,7 +21195,7 @@
         <v>451</v>
       </c>
       <c r="B15" t="s">
-        <v>398</v>
+        <v>452</v>
       </c>
       <c r="C15" t="s">
         <v>358</v>
@@ -21697,7 +21698,7 @@
         <v>451</v>
       </c>
       <c r="B16" t="s">
-        <v>399</v>
+        <v>453</v>
       </c>
       <c r="C16" t="s">
         <v>358</v>
@@ -22200,7 +22201,7 @@
         <v>451</v>
       </c>
       <c r="B17" t="s">
-        <v>400</v>
+        <v>454</v>
       </c>
       <c r="C17" t="s">
         <v>358</v>
@@ -22715,7 +22716,7 @@
       <selection pane="bottomLeft" activeCell="D14" sqref="A1:FR17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.44140625" style="24" bestFit="1" customWidth="1"/>
@@ -22784,7 +22785,7 @@
     <col min="173" max="174" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>166</v>
       </c>
@@ -23472,7 +23473,7 @@
         <v>عملکرد شغلی میانگین</v>
       </c>
     </row>
-    <row r="2" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="str">
         <f>'اطلاعات شخصی'!B2</f>
         <v>جناب آقای</v>
@@ -24170,7 +24171,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="3" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="str">
         <f>'اطلاعات شخصی'!B3</f>
         <v>جناب آقای</v>
@@ -24868,7 +24869,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="4" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="str">
         <f>'اطلاعات شخصی'!B4</f>
         <v>جناب آقای</v>
@@ -25566,7 +25567,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="5" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="str">
         <f>'اطلاعات شخصی'!B5</f>
         <v>جناب آقای</v>
@@ -26264,7 +26265,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="6" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="str">
         <f>'اطلاعات شخصی'!B6</f>
         <v>جناب آقای</v>
@@ -26962,7 +26963,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="7" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="str">
         <f>'اطلاعات شخصی'!B7</f>
         <v>جناب آقای</v>
@@ -27660,7 +27661,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="8" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="str">
         <f>'اطلاعات شخصی'!B8</f>
         <v>جناب آقای</v>
@@ -28358,7 +28359,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="9" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="str">
         <f>'اطلاعات شخصی'!B9</f>
         <v>سرکار خانم</v>
@@ -29056,7 +29057,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="10" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="str">
         <f>'اطلاعات شخصی'!B10</f>
         <v>سرکار خانم</v>
@@ -29754,7 +29755,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="11" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="str">
         <f>'اطلاعات شخصی'!B11</f>
         <v>سرکار خانم</v>
@@ -30452,7 +30453,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="12" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="str">
         <f>'اطلاعات شخصی'!B12</f>
         <v>سرکار خانم</v>
@@ -31150,7 +31151,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="13" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="str">
         <f>'اطلاعات شخصی'!B13</f>
         <v>سرکار خانم</v>
@@ -31848,7 +31849,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="14" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="str">
         <f>'اطلاعات شخصی'!B14</f>
         <v>سرکار خانم</v>
@@ -32546,7 +32547,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="15" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
         <v>175</v>
       </c>
@@ -33221,7 +33222,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="16" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>175</v>
       </c>
@@ -33896,7 +33897,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="17" spans="1:174" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:174" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
         <v>175</v>
       </c>
@@ -34585,7 +34586,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -34607,7 +34608,7 @@
     <col min="21" max="21" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -34688,7 +34689,7 @@
         <v>سن</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -34774,7 +34775,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -34860,7 +34861,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -34946,7 +34947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -35032,7 +35033,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -35118,7 +35119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -35204,7 +35205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -35290,7 +35291,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -35376,7 +35377,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -35462,7 +35463,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -35548,7 +35549,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -35634,7 +35635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -35720,7 +35721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -35806,7 +35807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -35848,7 +35849,7 @@
         <v>32.571428571428569</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -35890,7 +35891,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -35949,7 +35950,7 @@
       <selection pane="bottomLeft" activeCell="O2" sqref="O2:O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -35969,7 +35970,7 @@
     <col min="31" max="52" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -36141,7 +36142,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -36349,7 +36350,7 @@
         <v>1.5144298184855884</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -36557,7 +36558,7 @@
         <v>-0.90364087837562579</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -36765,7 +36766,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -36973,7 +36974,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -37181,7 +37182,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -37389,7 +37390,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -37597,7 +37598,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -37805,7 +37806,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="10" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -38013,7 +38014,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -38221,7 +38222,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -38429,7 +38430,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="13" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -38637,7 +38638,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -38845,7 +38846,7 @@
         <v>0.28113534146345742</v>
       </c>
     </row>
-    <row r="15" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -39053,7 +39054,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -39261,7 +39262,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="17" spans="1:52" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:52" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -39486,7 +39487,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -39500,7 +39501,7 @@
     <col min="15" max="34" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -39613,7 +39614,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -39751,7 +39752,7 @@
         <v>6.5392404513888902</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -39889,7 +39890,7 @@
         <v>8.603401562500002</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -40027,7 +40028,7 @@
         <v>7.2390820312500006</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -40165,7 +40166,7 @@
         <v>9.6439869791666659</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -40303,7 +40304,7 @@
         <v>7.2198833333333345</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -40441,7 +40442,7 @@
         <v>7.0661059027777791</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -40579,7 +40580,7 @@
         <v>8.0694848958333338</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -40717,7 +40718,7 @@
         <v>7.0389062847222226</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -40855,7 +40856,7 @@
         <v>6.4232503472222238</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -40993,7 +40994,7 @@
         <v>5.8348708333333326</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -41131,7 +41132,7 @@
         <v>5.5336291666666666</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -41269,7 +41270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -41407,7 +41408,7 @@
         <v>7.4666782986111109</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -41544,7 +41545,7 @@
         <v>9.1310507688492102</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -41681,7 +41682,7 @@
         <v>6.5945622251157419</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -41835,7 +41836,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -41854,7 +41855,7 @@
     <col min="44" max="55" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'اطلاعات شخصی'!B1</f>
         <v>جنسیت</v>
@@ -42050,7 +42051,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>'اطلاعات شخصی'!B2</f>
         <v>جناب آقای</v>
@@ -42272,7 +42273,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f>'اطلاعات شخصی'!B3</f>
         <v>جناب آقای</v>
@@ -42494,7 +42495,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f>'اطلاعات شخصی'!B4</f>
         <v>جناب آقای</v>
@@ -42716,7 +42717,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f>'اطلاعات شخصی'!B5</f>
         <v>جناب آقای</v>
@@ -42938,7 +42939,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f>'اطلاعات شخصی'!B6</f>
         <v>جناب آقای</v>
@@ -43160,7 +43161,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f>'اطلاعات شخصی'!B7</f>
         <v>جناب آقای</v>
@@ -43382,7 +43383,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="8" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f>'اطلاعات شخصی'!B8</f>
         <v>جناب آقای</v>
@@ -43604,7 +43605,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="9" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f>'اطلاعات شخصی'!B9</f>
         <v>سرکار خانم</v>
@@ -43826,7 +43827,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="10" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f>'اطلاعات شخصی'!B10</f>
         <v>سرکار خانم</v>
@@ -44048,7 +44049,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="11" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f>'اطلاعات شخصی'!B11</f>
         <v>سرکار خانم</v>
@@ -44270,7 +44271,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="12" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f>'اطلاعات شخصی'!B12</f>
         <v>سرکار خانم</v>
@@ -44492,7 +44493,7 @@
         <v>شدید</v>
       </c>
     </row>
-    <row r="13" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="str">
         <f>'اطلاعات شخصی'!B13</f>
         <v>سرکار خانم</v>
@@ -44714,7 +44715,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="14" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f>'اطلاعات شخصی'!B14</f>
         <v>سرکار خانم</v>
@@ -44936,7 +44937,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="15" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'اطلاعات شخصی'!B15</f>
         <v>7</v>
@@ -45158,7 +45159,7 @@
         <v>14.285714285714285</v>
       </c>
     </row>
-    <row r="16" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'اطلاعات شخصی'!B16</f>
         <v>6</v>
@@ -45380,7 +45381,7 @@
         <v>16.666666666666664</v>
       </c>
     </row>
-    <row r="17" spans="1:55" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'اطلاعات شخصی'!B17</f>
         <v>13</v>
@@ -45616,7 +45617,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
@@ -45651,7 +45652,7 @@
     <col min="83" max="88" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="str">
         <f>'داده ها'!A1</f>
         <v>جنسیت عدد</v>
@@ -45963,7 +45964,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <f>'داده ها'!A2</f>
         <v>2</v>
@@ -46317,7 +46318,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="3" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <f>'داده ها'!A3</f>
         <v>2</v>
@@ -46671,7 +46672,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="4" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <f>'داده ها'!A4</f>
         <v>2</v>
@@ -47025,7 +47026,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="5" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <f>'داده ها'!A5</f>
         <v>2</v>
@@ -47379,7 +47380,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="6" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <f>'داده ها'!A6</f>
         <v>2</v>
@@ -47733,7 +47734,7 @@
         <v>شدید</v>
       </c>
     </row>
-    <row r="7" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <f>'داده ها'!A7</f>
         <v>2</v>
@@ -48087,7 +48088,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="8" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <f>'داده ها'!A8</f>
         <v>2</v>
@@ -48441,7 +48442,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="9" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <f>'داده ها'!A9</f>
         <v>1</v>
@@ -48795,7 +48796,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="10" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <f>'داده ها'!A10</f>
         <v>1</v>
@@ -49149,7 +49150,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="11" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <f>'داده ها'!A11</f>
         <v>1</v>
@@ -49503,7 +49504,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="12" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <f>'داده ها'!A12</f>
         <v>1</v>
@@ -49857,7 +49858,7 @@
         <v>طبیعی</v>
       </c>
     </row>
-    <row r="13" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <f>'داده ها'!A13</f>
         <v>1</v>
@@ -50211,7 +50212,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="14" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <f>'داده ها'!A14</f>
         <v>1</v>
@@ -50565,7 +50566,7 @@
         <v>خفیف</v>
       </c>
     </row>
-    <row r="15" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <f>'داده ها'!A15</f>
         <v>2</v>
@@ -50919,7 +50920,7 @@
         <v>71.428571428571431</v>
       </c>
     </row>
-    <row r="16" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <f>'داده ها'!A16</f>
         <v>1</v>
@@ -51273,7 +51274,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:88" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:88" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <f>'داده ها'!A17</f>
         <v>0</v>
@@ -51644,7 +51645,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -51675,7 +51676,7 @@
     <col min="179" max="180" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="str">
         <f>'داده ها'!CO1</f>
         <v>A1</v>
@@ -52354,7 +52355,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D2" s="5">
         <f>'داده ها'!CO2</f>
         <v>0</v>
@@ -53064,7 +53065,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="3" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D3" s="5">
         <f>'داده ها'!CO3</f>
         <v>0</v>
@@ -53774,7 +53775,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="4" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="5">
         <f>'داده ها'!CO4</f>
         <v>0</v>
@@ -54484,7 +54485,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="5" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D5" s="5">
         <f>'داده ها'!CO5</f>
         <v>0</v>
@@ -55194,7 +55195,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="6" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D6" s="5">
         <f>'داده ها'!CO6</f>
         <v>0</v>
@@ -55904,7 +55905,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="7" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D7" s="5">
         <f>'داده ها'!CO7</f>
         <v>0</v>
@@ -56614,7 +56615,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="8" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="5">
         <f>'داده ها'!CO8</f>
         <v>0</v>
@@ -57324,7 +57325,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="9" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="5">
         <f>'داده ها'!CO9</f>
         <v>0</v>
@@ -58034,7 +58035,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="10" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D10" s="5">
         <f>'داده ها'!CO10</f>
         <v>0</v>
@@ -58744,7 +58745,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="11" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D11" s="5">
         <f>'داده ها'!CO11</f>
         <v>0</v>
@@ -59454,7 +59455,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="12" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" s="5">
         <f>'داده ها'!CO12</f>
         <v>0</v>
@@ -60164,7 +60165,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="13" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5">
         <f>'داده ها'!CO13</f>
         <v>0</v>
@@ -60874,7 +60875,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="14" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D14" s="5">
         <f>'داده ها'!CO14</f>
         <v>0</v>
@@ -61584,7 +61585,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="15" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D15" s="5">
         <f t="shared" ref="D15:K15" si="31">AVERAGE(D2:D8)</f>
         <v>0</v>
@@ -62294,7 +62295,7 @@
         <v>بهتر از متوسط</v>
       </c>
     </row>
-    <row r="16" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D16" s="5">
         <f t="shared" ref="D16:K16" si="38">AVERAGE(D9:D14)</f>
         <v>0</v>
@@ -63004,7 +63005,7 @@
         <v>بدتر از متوسط</v>
       </c>
     </row>
-    <row r="17" spans="4:180" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:180" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D17" s="5">
         <f t="shared" ref="D17:K17" si="45">AVERAGE(D2:D14)</f>
         <v>0</v>

</xml_diff>